<commit_message>
Update Ops Dec 2023
Update Ops Dec 2023
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2023-12.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2023-12.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1844BB02-27AE-4635-A30E-EAAC5ED8EA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD37617-DAF7-4FF2-8373-D6D6149A5B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="6" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
@@ -86,24 +86,6 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={9982AFAF-E6E7-45BF-A44A-0C0167B0574C}</author>
-  </authors>
-  <commentList>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{9982AFAF-E6E7-45BF-A44A-0C0167B0574C}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    1) Redox</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
     <author>tc={4EE09740-4AB8-4767-BD8A-38F7D58F39B2}</author>
   </authors>
   <commentList>
@@ -119,7 +101,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={77BE6F65-1B38-40C6-BD39-81B5DFEC0749}</author>
@@ -138,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="213">
   <si>
     <t>Course</t>
   </si>
@@ -605,10 +587,6 @@
 Timing: Friday 4-6pm     ||     Start date: 22/Sep/2023</t>
   </si>
   <si>
-    <t>Faculty: Subrata Ghosh     ||     Batch: B2: Booster JELET Crash Course Chemistry
-Timing: Thursday 2-6pm     ||     Start date: 07/Sep/2023</t>
-  </si>
-  <si>
     <t>Faculty: Subrata Ghosh     ||     Batch: B1: NEET &amp; IIT Crash Course Chemistry
 Timing: Thursday 4-6pm     ||     Start date: 07/Sep/2023</t>
   </si>
@@ -758,6 +736,34 @@
   </si>
   <si>
     <t>On Going</t>
+  </si>
+  <si>
+    <t>Faculty: Avishek Adhikari     ||     Batch: B2: Booster JELET Crash Course Chemistry
+Timing: Thursday 2-6pm     ||     Start date: 07/Sep/2023</t>
+  </si>
+  <si>
+    <t>10:30 PM - 12:30 PM</t>
+  </si>
+  <si>
+    <t>1) Oscillation &amp; Waves</t>
+  </si>
+  <si>
+    <t>12:30 PM - 2:00 PM</t>
+  </si>
+  <si>
+    <t>1) Vector</t>
+  </si>
+  <si>
+    <t>2) Straight Line</t>
+  </si>
+  <si>
+    <t>2:00 PM - 03:00 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Nomenclature </t>
+  </si>
+  <si>
+    <t>of Organic Chemistry</t>
   </si>
 </sst>
 </file>
@@ -1529,7 +1535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1922,10 +1928,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2267,21 +2269,13 @@
 
 <file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D12" dT="2023-11-02T12:47:03.22" personId="{A98E9D41-33A5-4BF6-BDEF-83BD84C6E107}" id="{9982AFAF-E6E7-45BF-A44A-0C0167B0574C}">
-    <text>1) Redox</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="D12" dT="2023-11-04T08:33:38.77" personId="{A98E9D41-33A5-4BF6-BDEF-83BD84C6E107}" id="{4EE09740-4AB8-4767-BD8A-38F7D58F39B2}">
     <text>1) Elasticity</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="D12" dT="2023-11-04T08:34:55.19" personId="{A98E9D41-33A5-4BF6-BDEF-83BD84C6E107}" id="{77BE6F65-1B38-40C6-BD39-81B5DFEC0749}">
     <text>1) Determinants</text>
@@ -3421,19 +3415,19 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G15" s="1">
         <v>10000</v>
@@ -3450,7 +3444,7 @@
         <v>45234</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
@@ -4078,7 +4072,7 @@
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="155" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="156"/>
       <c r="D2" s="156"/>
@@ -4092,7 +4086,7 @@
         <v>148</v>
       </c>
       <c r="O2" s="126" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P2" s="65" t="s">
         <v>8</v>
@@ -4555,7 +4549,7 @@
     <row r="31" spans="13:16" x14ac:dyDescent="0.3">
       <c r="M31" s="97"/>
       <c r="N31" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O31" s="126">
         <f>SUM(O4:O29)</f>
@@ -4577,7 +4571,7 @@
     <row r="33" spans="13:16" x14ac:dyDescent="0.3">
       <c r="M33" s="97"/>
       <c r="N33" s="65" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O33" s="126">
         <f>ROUND((O31/O32)*100,2)</f>
@@ -4599,17 +4593,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A980A2-087E-4BDA-864D-B7CC763A9F65}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A980A2-087E-4BDA-864D-B7CC763A9F65}">
   <dimension ref="B1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
@@ -4621,7 +4615,7 @@
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="155" t="s">
-        <v>154</v>
+        <v>204</v>
       </c>
       <c r="C2" s="156"/>
       <c r="D2" s="156"/>
@@ -4635,7 +4629,7 @@
         <v>148</v>
       </c>
       <c r="O2" s="126" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P2" s="65" t="s">
         <v>8</v>
@@ -4666,7 +4660,9 @@
       <c r="C4" s="163" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="129">
+        <v>45269</v>
+      </c>
       <c r="E4" s="38"/>
       <c r="F4" s="38"/>
       <c r="G4" s="49"/>
@@ -4678,7 +4674,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="63" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O4" s="97">
         <v>0</v>
@@ -4688,7 +4684,9 @@
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="162"/>
       <c r="C5" s="164"/>
-      <c r="D5" s="39"/>
+      <c r="D5" s="62" t="s">
+        <v>210</v>
+      </c>
       <c r="E5" s="39"/>
       <c r="F5" s="66"/>
       <c r="G5" s="66"/>
@@ -4700,7 +4698,7 @@
         <v>2</v>
       </c>
       <c r="N5" s="125" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O5" s="124">
         <v>1</v>
@@ -4714,7 +4712,9 @@
       <c r="C6" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="40"/>
+      <c r="D6" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="E6" s="41"/>
       <c r="F6" s="41"/>
       <c r="G6" s="41"/>
@@ -4726,7 +4726,7 @@
         <v>3</v>
       </c>
       <c r="N6" s="63" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O6" s="97">
         <v>0</v>
@@ -4746,13 +4746,13 @@
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
       <c r="K7" s="44"/>
-      <c r="M7" s="182">
+      <c r="M7" s="97">
         <v>4</v>
       </c>
-      <c r="N7" s="183" t="s">
-        <v>166</v>
-      </c>
-      <c r="O7" s="182">
+      <c r="N7" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="O7" s="97">
         <v>0</v>
       </c>
       <c r="P7" s="63"/>
@@ -4774,7 +4774,7 @@
         <v>5</v>
       </c>
       <c r="N8" s="63" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O8" s="97">
         <v>0</v>
@@ -4798,7 +4798,7 @@
         <v>6</v>
       </c>
       <c r="N9" s="63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O9" s="97">
         <v>0</v>
@@ -4822,7 +4822,7 @@
         <v>7</v>
       </c>
       <c r="N10" s="63" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O10" s="97">
         <v>0</v>
@@ -4846,7 +4846,7 @@
         <v>8</v>
       </c>
       <c r="N11" s="63" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O11" s="97">
         <v>0</v>
@@ -4858,7 +4858,9 @@
         <v>59</v>
       </c>
       <c r="C12" s="169"/>
-      <c r="D12" s="127"/>
+      <c r="D12" s="127" t="s">
+        <v>211</v>
+      </c>
       <c r="E12" s="63"/>
       <c r="F12" s="63"/>
       <c r="G12" s="63"/>
@@ -4870,13 +4872,15 @@
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="63"/>
       <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
+      <c r="D13" s="63" t="s">
+        <v>212</v>
+      </c>
       <c r="E13" s="63"/>
       <c r="F13" s="63"/>
       <c r="G13" s="63"/>
       <c r="M13" s="97"/>
       <c r="N13" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O13" s="126">
         <f>SUM(O4:O11)</f>
@@ -4904,7 +4908,7 @@
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="M15" s="97"/>
       <c r="N15" s="65" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O15" s="126">
         <f>ROUND((O13/O14)*100,2)</f>
@@ -4925,7 +4929,6 @@
     <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4933,8 +4936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DABE7A-7845-46EA-BB0E-44CB73A3B0F1}">
   <dimension ref="B1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4973,7 +4976,7 @@
         <v>148</v>
       </c>
       <c r="P2" s="99" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q2" s="98" t="s">
         <v>8</v>
@@ -4989,7 +4992,7 @@
       <c r="H3" s="177"/>
       <c r="I3" s="178"/>
       <c r="J3" s="165" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K3" s="166"/>
       <c r="L3" s="167"/>
@@ -5011,7 +5014,9 @@
       <c r="E4" s="129">
         <v>45265</v>
       </c>
-      <c r="F4" s="129"/>
+      <c r="F4" s="129">
+        <v>45269</v>
+      </c>
       <c r="G4" s="130"/>
       <c r="H4" s="130"/>
       <c r="I4" s="149"/>
@@ -5022,7 +5027,7 @@
         <v>1</v>
       </c>
       <c r="O4" s="125" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P4" s="124">
         <v>1</v>
@@ -5038,7 +5043,9 @@
       <c r="E5" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="62"/>
+      <c r="F5" s="62" t="s">
+        <v>205</v>
+      </c>
       <c r="G5" s="62"/>
       <c r="H5" s="62"/>
       <c r="I5" s="148"/>
@@ -5049,7 +5056,7 @@
         <v>2</v>
       </c>
       <c r="O5" s="125" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P5" s="124">
         <v>1</v>
@@ -5069,7 +5076,9 @@
       <c r="E6" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="40"/>
+      <c r="F6" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="G6" s="40"/>
       <c r="H6" s="40"/>
       <c r="I6" s="150"/>
@@ -5080,13 +5089,13 @@
         <v>3</v>
       </c>
       <c r="O6" s="63" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P6" s="97">
         <v>0</v>
       </c>
       <c r="Q6" s="63" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
@@ -5107,7 +5116,7 @@
         <v>4</v>
       </c>
       <c r="O7" s="125" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P7" s="124">
         <v>1</v>
@@ -5132,7 +5141,7 @@
         <v>5</v>
       </c>
       <c r="O8" s="63" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="P8" s="97">
         <v>0</v>
@@ -5157,7 +5166,7 @@
         <v>6</v>
       </c>
       <c r="O9" s="125" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P9" s="124">
         <v>1</v>
@@ -5182,7 +5191,7 @@
         <v>7</v>
       </c>
       <c r="O10" s="125" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P10" s="124">
         <v>1</v>
@@ -5207,7 +5216,7 @@
         <v>8</v>
       </c>
       <c r="O11" s="125" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P11" s="124">
         <v>1</v>
@@ -5220,12 +5229,14 @@
       </c>
       <c r="C12" s="160"/>
       <c r="D12" s="63" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E12" s="63" t="s">
-        <v>203</v>
-      </c>
-      <c r="F12" s="63"/>
+        <v>202</v>
+      </c>
+      <c r="F12" s="63" t="s">
+        <v>206</v>
+      </c>
       <c r="G12" s="63"/>
       <c r="H12" s="63"/>
       <c r="I12" s="34"/>
@@ -5236,7 +5247,7 @@
         <v>9</v>
       </c>
       <c r="O12" s="63" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P12" s="97">
         <v>0</v>
@@ -5259,7 +5270,7 @@
         <v>10</v>
       </c>
       <c r="O13" s="63" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P13" s="97">
         <v>0</v>
@@ -5305,7 +5316,7 @@
         <v>12</v>
       </c>
       <c r="O15" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P15" s="97">
         <v>0</v>
@@ -5317,7 +5328,7 @@
         <v>13</v>
       </c>
       <c r="O16" s="63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P16" s="97">
         <v>0</v>
@@ -5329,7 +5340,7 @@
         <v>14</v>
       </c>
       <c r="O17" s="63" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P17" s="97">
         <v>0</v>
@@ -5341,7 +5352,7 @@
         <v>15</v>
       </c>
       <c r="O18" s="63" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P18" s="97">
         <v>0</v>
@@ -5351,7 +5362,7 @@
     <row r="21" spans="12:17" x14ac:dyDescent="0.3">
       <c r="N21" s="97"/>
       <c r="O21" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P21" s="126">
         <f>SUM(P4:P15)</f>
@@ -5373,7 +5384,7 @@
     <row r="23" spans="12:17" x14ac:dyDescent="0.3">
       <c r="N23" s="97"/>
       <c r="O23" s="65" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P23" s="126">
         <f>ROUND((P21/P22)*100,2)</f>
@@ -5404,7 +5415,7 @@
   <dimension ref="B1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5440,7 +5451,7 @@
         <v>148</v>
       </c>
       <c r="O2" s="99" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P2" s="98" t="s">
         <v>8</v>
@@ -5475,7 +5486,9 @@
       <c r="E4" s="129">
         <v>45265</v>
       </c>
-      <c r="F4" s="129"/>
+      <c r="F4" s="129">
+        <v>45269</v>
+      </c>
       <c r="G4" s="130"/>
       <c r="H4" s="130"/>
       <c r="I4" s="145"/>
@@ -5485,7 +5498,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="125" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O4" s="124">
         <v>1</v>
@@ -5496,12 +5509,14 @@
       <c r="B5" s="162"/>
       <c r="C5" s="164"/>
       <c r="D5" s="62" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E5" s="62" t="s">
-        <v>200</v>
-      </c>
-      <c r="F5" s="62"/>
+        <v>199</v>
+      </c>
+      <c r="F5" s="62" t="s">
+        <v>207</v>
+      </c>
       <c r="G5" s="62"/>
       <c r="H5" s="62"/>
       <c r="I5" s="146"/>
@@ -5511,7 +5526,7 @@
         <v>2</v>
       </c>
       <c r="N5" s="125" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O5" s="124">
         <v>1</v>
@@ -5531,7 +5546,9 @@
       <c r="E6" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="40"/>
+      <c r="F6" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="G6" s="40"/>
       <c r="H6" s="40"/>
       <c r="I6" s="42"/>
@@ -5541,7 +5558,7 @@
         <v>3</v>
       </c>
       <c r="N6" s="125" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O6" s="124">
         <v>1</v>
@@ -5565,13 +5582,13 @@
         <v>4</v>
       </c>
       <c r="N7" s="63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O7" s="97">
         <v>0</v>
       </c>
       <c r="P7" s="63" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
@@ -5591,7 +5608,7 @@
         <v>5</v>
       </c>
       <c r="N8" s="125" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O8" s="124">
         <v>1</v>
@@ -5615,7 +5632,7 @@
         <v>6</v>
       </c>
       <c r="N9" s="63" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O9" s="97">
         <v>0</v>
@@ -5639,7 +5656,7 @@
         <v>7</v>
       </c>
       <c r="N10" s="63" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O10" s="97">
         <v>0</v>
@@ -5663,7 +5680,7 @@
         <v>8</v>
       </c>
       <c r="N11" s="63" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O11" s="97">
         <v>0</v>
@@ -5676,12 +5693,14 @@
       </c>
       <c r="C12" s="160"/>
       <c r="D12" s="63" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E12" s="63" t="s">
-        <v>201</v>
-      </c>
-      <c r="F12" s="63"/>
+        <v>200</v>
+      </c>
+      <c r="F12" s="63" t="s">
+        <v>208</v>
+      </c>
       <c r="G12" s="63"/>
       <c r="H12" s="63"/>
       <c r="I12" s="128"/>
@@ -5691,7 +5710,7 @@
         <v>9</v>
       </c>
       <c r="N12" s="63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O12" s="97">
         <v>0</v>
@@ -5703,7 +5722,9 @@
       <c r="C13" s="63"/>
       <c r="D13" s="63"/>
       <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
+      <c r="F13" s="63" t="s">
+        <v>209</v>
+      </c>
       <c r="G13" s="63"/>
       <c r="H13" s="63"/>
       <c r="I13" s="128"/>
@@ -5713,7 +5734,7 @@
         <v>10</v>
       </c>
       <c r="N13" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O13" s="97">
         <v>0</v>
@@ -5735,7 +5756,7 @@
         <v>11</v>
       </c>
       <c r="N14" s="63" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O14" s="97">
         <v>0</v>
@@ -5757,7 +5778,7 @@
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="M16" s="97"/>
       <c r="N16" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O16" s="126">
         <f>SUM(O4:O14)</f>
@@ -5779,7 +5800,7 @@
     <row r="18" spans="13:16" x14ac:dyDescent="0.3">
       <c r="M18" s="97"/>
       <c r="N18" s="65" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O18" s="126">
         <f>ROUND((O16/O17)*100,2)</f>

</xml_diff>

<commit_message>
Ops of December 2023
Ops of December 2023
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2023-12.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2023-12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B74CACB-9766-431A-AC5F-D385E33A83F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F440593-7169-49DA-B698-0097B9453BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="8" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="6" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="226">
   <si>
     <t>Course</t>
   </si>
@@ -788,6 +788,21 @@
   </si>
   <si>
     <t>for Maths</t>
+  </si>
+  <si>
+    <t>1) Structure of Atoms</t>
+  </si>
+  <si>
+    <t>Doubt clearance on</t>
+  </si>
+  <si>
+    <t>numericals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doubt clearing on vector </t>
+  </si>
+  <si>
+    <t>algebra</t>
   </si>
 </sst>
 </file>
@@ -977,7 +992,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1521,19 +1536,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -1544,7 +1546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1829,18 +1831,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1922,9 +1913,31 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2363,14 +2376,14 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="147" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="152"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="149"/>
       <c r="M2" s="97" t="s">
         <v>147</v>
       </c>
@@ -2388,18 +2401,18 @@
       </c>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="153"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="154"/>
-      <c r="E3" s="154"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="160" t="s">
+      <c r="B3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="157" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="162"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="159"/>
       <c r="M3" s="62"/>
       <c r="N3" s="96"/>
       <c r="O3" s="62"/>
@@ -2407,10 +2420,10 @@
       <c r="Q3" s="62"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="153" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="158" t="s">
+      <c r="C4" s="155" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="37"/>
@@ -2436,8 +2449,8 @@
       <c r="Q4" s="62"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="157"/>
-      <c r="C5" s="159"/>
+      <c r="B5" s="154"/>
+      <c r="C5" s="156"/>
       <c r="D5" s="65"/>
       <c r="E5" s="65"/>
       <c r="F5" s="65"/>
@@ -2611,10 +2624,10 @@
       <c r="Q11" s="62"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="155" t="s">
+      <c r="B12" s="152" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="155"/>
+      <c r="C12" s="152"/>
       <c r="D12" s="94"/>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
@@ -4069,14 +4082,14 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="147" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="152"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="149"/>
       <c r="M2" s="125" t="s">
         <v>145</v>
       </c>
@@ -4091,28 +4104,28 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="153"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="154"/>
-      <c r="E3" s="154"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="160" t="s">
+      <c r="B3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="157" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="162"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="159"/>
       <c r="M3" s="96"/>
       <c r="N3" s="62"/>
       <c r="O3" s="96"/>
       <c r="P3" s="62"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="153" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="158" t="s">
+      <c r="C4" s="155" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="37"/>
@@ -4135,8 +4148,8 @@
       <c r="P4" s="62"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="157"/>
-      <c r="C5" s="159"/>
+      <c r="B5" s="154"/>
+      <c r="C5" s="156"/>
       <c r="D5" s="65"/>
       <c r="E5" s="65"/>
       <c r="F5" s="65"/>
@@ -4303,10 +4316,10 @@
       <c r="P11" s="62"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="155" t="s">
+      <c r="B12" s="152" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="155"/>
+      <c r="C12" s="152"/>
       <c r="D12" s="62"/>
       <c r="E12" s="62"/>
       <c r="F12" s="62"/>
@@ -4592,10 +4605,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A980A2-087E-4BDA-864D-B7CC763A9F65}">
-  <dimension ref="B1:P16"/>
+  <dimension ref="B1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4603,58 +4616,61 @@
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="45.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="150" t="s">
+    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="152"/>
-      <c r="M2" s="125" t="s">
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="149"/>
+      <c r="N2" s="125" t="s">
         <v>145</v>
       </c>
-      <c r="N2" s="64" t="s">
+      <c r="O2" s="64" t="s">
         <v>148</v>
       </c>
-      <c r="O2" s="125" t="s">
+      <c r="P2" s="125" t="s">
         <v>160</v>
       </c>
-      <c r="P2" s="64" t="s">
+      <c r="Q2" s="64" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="153"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="154"/>
-      <c r="E3" s="154"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="160" t="s">
+    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="157" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="162"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="96"/>
-      <c r="P3" s="62"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="156" t="s">
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
+      <c r="L3" s="159"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="96"/>
+      <c r="Q3" s="62"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="153" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="158" t="s">
+      <c r="C4" s="155" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="128">
@@ -4669,24 +4685,27 @@
       <c r="G4" s="128">
         <v>45279</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="56"/>
+      <c r="H4" s="128">
+        <v>45286</v>
+      </c>
+      <c r="I4" s="55"/>
       <c r="J4" s="56"/>
-      <c r="K4" s="57"/>
-      <c r="M4" s="96">
+      <c r="K4" s="56"/>
+      <c r="L4" s="57"/>
+      <c r="N4" s="96">
         <v>1</v>
       </c>
-      <c r="N4" s="62" t="s">
+      <c r="O4" s="62" t="s">
         <v>162</v>
       </c>
-      <c r="O4" s="96">
-        <v>0</v>
-      </c>
-      <c r="P4" s="62"/>
-    </row>
-    <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="157"/>
-      <c r="C5" s="159"/>
+      <c r="P4" s="96">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="62"/>
+    </row>
+    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="154"/>
+      <c r="C5" s="156"/>
       <c r="D5" s="61" t="s">
         <v>207</v>
       </c>
@@ -4699,22 +4718,25 @@
       <c r="G5" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="59"/>
+      <c r="H5" s="61" t="s">
+        <v>207</v>
+      </c>
+      <c r="I5" s="58"/>
       <c r="J5" s="59"/>
-      <c r="K5" s="60"/>
-      <c r="M5" s="123">
+      <c r="K5" s="59"/>
+      <c r="L5" s="60"/>
+      <c r="N5" s="123">
         <v>2</v>
       </c>
-      <c r="N5" s="124" t="s">
+      <c r="O5" s="124" t="s">
         <v>163</v>
       </c>
-      <c r="O5" s="123">
+      <c r="P5" s="123">
         <v>1</v>
       </c>
-      <c r="P5" s="62"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="Q5" s="62"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="31">
         <v>1</v>
       </c>
@@ -4733,22 +4755,25 @@
       <c r="G6" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="52"/>
-      <c r="I6" s="53"/>
+      <c r="H6" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="52"/>
       <c r="J6" s="53"/>
-      <c r="K6" s="54"/>
-      <c r="M6" s="96">
+      <c r="K6" s="53"/>
+      <c r="L6" s="54"/>
+      <c r="N6" s="96">
         <v>3</v>
       </c>
-      <c r="N6" s="62" t="s">
+      <c r="O6" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="O6" s="96">
-        <v>0</v>
-      </c>
-      <c r="P6" s="62"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P6" s="96">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="62"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="33">
         <v>2</v>
       </c>
@@ -4757,22 +4782,23 @@
       <c r="E7" s="42"/>
       <c r="F7" s="42"/>
       <c r="G7" s="49"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="42"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="50"/>
       <c r="J7" s="42"/>
-      <c r="K7" s="43"/>
-      <c r="M7" s="96">
+      <c r="K7" s="42"/>
+      <c r="L7" s="43"/>
+      <c r="N7" s="96">
         <v>4</v>
       </c>
-      <c r="N7" s="62" t="s">
+      <c r="O7" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="O7" s="96">
-        <v>0</v>
-      </c>
-      <c r="P7" s="62"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P7" s="96">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="62"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="33">
         <v>3</v>
       </c>
@@ -4781,22 +4807,23 @@
       <c r="E8" s="42"/>
       <c r="F8" s="42"/>
       <c r="G8" s="49"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="42"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="50"/>
       <c r="J8" s="42"/>
-      <c r="K8" s="43"/>
-      <c r="M8" s="96">
+      <c r="K8" s="42"/>
+      <c r="L8" s="43"/>
+      <c r="N8" s="123">
         <v>5</v>
       </c>
-      <c r="N8" s="62" t="s">
+      <c r="O8" s="124" t="s">
         <v>166</v>
       </c>
-      <c r="O8" s="96">
-        <v>0</v>
-      </c>
-      <c r="P8" s="62"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P8" s="123">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="62"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="33">
         <v>4</v>
       </c>
@@ -4805,22 +4832,23 @@
       <c r="E9" s="42"/>
       <c r="F9" s="42"/>
       <c r="G9" s="49"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="42"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
       <c r="J9" s="42"/>
-      <c r="K9" s="43"/>
-      <c r="M9" s="96">
+      <c r="K9" s="42"/>
+      <c r="L9" s="43"/>
+      <c r="N9" s="96">
         <v>6</v>
       </c>
-      <c r="N9" s="62" t="s">
+      <c r="O9" s="62" t="s">
         <v>167</v>
       </c>
-      <c r="O9" s="96">
-        <v>0</v>
-      </c>
-      <c r="P9" s="62"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P9" s="96">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="62"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="33">
         <v>5</v>
       </c>
@@ -4829,22 +4857,23 @@
       <c r="E10" s="42"/>
       <c r="F10" s="42"/>
       <c r="G10" s="49"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="42"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
       <c r="J10" s="42"/>
-      <c r="K10" s="43"/>
-      <c r="M10" s="96">
+      <c r="K10" s="42"/>
+      <c r="L10" s="43"/>
+      <c r="N10" s="96">
         <v>7</v>
       </c>
-      <c r="N10" s="62" t="s">
+      <c r="O10" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="O10" s="96">
-        <v>0</v>
-      </c>
-      <c r="P10" s="62"/>
-    </row>
-    <row r="11" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P10" s="96">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="62"/>
+    </row>
+    <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="35">
         <v>6</v>
       </c>
@@ -4853,26 +4882,27 @@
       <c r="E11" s="45"/>
       <c r="F11" s="45"/>
       <c r="G11" s="108"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="45"/>
+      <c r="H11" s="108"/>
+      <c r="I11" s="51"/>
       <c r="J11" s="45"/>
-      <c r="K11" s="46"/>
-      <c r="M11" s="96">
+      <c r="K11" s="45"/>
+      <c r="L11" s="46"/>
+      <c r="N11" s="96">
         <v>8</v>
       </c>
-      <c r="N11" s="62" t="s">
+      <c r="O11" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="O11" s="96">
-        <v>0</v>
-      </c>
-      <c r="P11" s="62"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="163" t="s">
+      <c r="P11" s="96">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="62"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="160" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="164"/>
+      <c r="C12" s="161"/>
       <c r="D12" s="126" t="s">
         <v>208</v>
       </c>
@@ -4885,12 +4915,15 @@
       <c r="G12" s="62" t="s">
         <v>210</v>
       </c>
-      <c r="M12" s="96"/>
-      <c r="N12" s="62"/>
-      <c r="O12" s="96"/>
-      <c r="P12" s="62"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H12" s="62" t="s">
+        <v>221</v>
+      </c>
+      <c r="N12" s="96"/>
+      <c r="O12" s="62"/>
+      <c r="P12" s="96"/>
+      <c r="Q12" s="62"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="62"/>
       <c r="C13" s="62"/>
       <c r="D13" s="62" t="s">
@@ -4899,52 +4932,54 @@
       <c r="E13" s="62"/>
       <c r="F13" s="62"/>
       <c r="G13" s="62"/>
-      <c r="M13" s="96"/>
-      <c r="N13" s="64" t="s">
+      <c r="H13" s="62"/>
+      <c r="N13" s="96"/>
+      <c r="O13" s="64" t="s">
         <v>161</v>
       </c>
-      <c r="O13" s="125">
-        <f>SUM(O4:O11)</f>
-        <v>1</v>
-      </c>
-      <c r="P13" s="62"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P13" s="125">
+        <f>SUM(P4:P11)</f>
+        <v>2</v>
+      </c>
+      <c r="Q13" s="62"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="62"/>
       <c r="C14" s="62"/>
       <c r="D14" s="62"/>
       <c r="E14" s="62"/>
       <c r="F14" s="62"/>
       <c r="G14" s="62"/>
-      <c r="M14" s="96"/>
-      <c r="N14" s="64" t="s">
+      <c r="H14" s="62"/>
+      <c r="N14" s="96"/>
+      <c r="O14" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="O14" s="125">
-        <f>COUNT(O4:O11)</f>
+      <c r="P14" s="125">
+        <f>COUNT(P4:P11)</f>
         <v>8</v>
       </c>
-      <c r="P14" s="62"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="M15" s="96"/>
-      <c r="N15" s="64" t="s">
+      <c r="Q14" s="62"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N15" s="96"/>
+      <c r="O15" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="O15" s="125">
-        <f>ROUND((O13/O14)*100,2)</f>
-        <v>12.5</v>
-      </c>
-      <c r="P15" s="62"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="M16" s="95"/>
-      <c r="O16" s="95"/>
+      <c r="P15" s="125">
+        <f>ROUND((P13/P14)*100,2)</f>
+        <v>25</v>
+      </c>
+      <c r="Q15" s="62"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N16" s="95"/>
+      <c r="P16" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="I3:L3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B12:C12"/>
@@ -4955,10 +4990,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DABE7A-7845-46EA-BB0E-44CB73A3B0F1}">
-  <dimension ref="B1:Q24"/>
+  <dimension ref="B1:R24"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4969,63 +5004,66 @@
     <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="168" t="s">
+    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="165" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="170"/>
-      <c r="N2" s="98" t="s">
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
+      <c r="G2" s="166"/>
+      <c r="H2" s="166"/>
+      <c r="I2" s="175"/>
+      <c r="J2" s="167"/>
+      <c r="O2" s="98" t="s">
         <v>145</v>
       </c>
-      <c r="O2" s="97" t="s">
+      <c r="P2" s="97" t="s">
         <v>148</v>
       </c>
-      <c r="P2" s="98" t="s">
+      <c r="Q2" s="98" t="s">
         <v>160</v>
       </c>
-      <c r="Q2" s="97" t="s">
+      <c r="R2" s="97" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="171"/>
-      <c r="C3" s="172"/>
-      <c r="D3" s="172"/>
-      <c r="E3" s="172"/>
-      <c r="F3" s="172"/>
-      <c r="G3" s="172"/>
-      <c r="H3" s="172"/>
-      <c r="I3" s="173"/>
-      <c r="J3" s="160" t="s">
+    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="168"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="176"/>
+      <c r="J3" s="170"/>
+      <c r="K3" s="157" t="s">
         <v>200</v>
       </c>
-      <c r="K3" s="161"/>
-      <c r="L3" s="162"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="96"/>
-      <c r="Q3" s="62"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="165" t="s">
+      <c r="L3" s="158"/>
+      <c r="M3" s="159"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="96"/>
+      <c r="R3" s="62"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="162" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="166" t="s">
+      <c r="C4" s="163" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="128">
@@ -5043,26 +5081,29 @@
       <c r="H4" s="128">
         <v>45276</v>
       </c>
-      <c r="I4" s="128">
+      <c r="I4" s="182">
         <v>45279</v>
       </c>
-      <c r="J4" s="147"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="116"/>
-      <c r="N4" s="123">
+      <c r="J4" s="182">
+        <v>45286</v>
+      </c>
+      <c r="K4" s="179"/>
+      <c r="L4" s="115"/>
+      <c r="M4" s="116"/>
+      <c r="O4" s="123">
         <v>1</v>
       </c>
-      <c r="O4" s="124" t="s">
+      <c r="P4" s="124" t="s">
         <v>180</v>
       </c>
-      <c r="P4" s="123">
+      <c r="Q4" s="123">
         <v>1</v>
       </c>
-      <c r="Q4" s="124"/>
-    </row>
-    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="157"/>
-      <c r="C5" s="159"/>
+      <c r="R4" s="124"/>
+    </row>
+    <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="154"/>
+      <c r="C5" s="156"/>
       <c r="D5" s="61" t="s">
         <v>49</v>
       </c>
@@ -5078,24 +5119,27 @@
       <c r="H5" s="61" t="s">
         <v>203</v>
       </c>
-      <c r="I5" s="61" t="s">
+      <c r="I5" s="183" t="s">
         <v>203</v>
       </c>
-      <c r="J5" s="148"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="60"/>
-      <c r="N5" s="123">
+      <c r="J5" s="183" t="s">
+        <v>203</v>
+      </c>
+      <c r="K5" s="180"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="60"/>
+      <c r="O5" s="123">
         <v>2</v>
       </c>
-      <c r="O5" s="124" t="s">
+      <c r="P5" s="124" t="s">
         <v>181</v>
       </c>
-      <c r="P5" s="123">
+      <c r="Q5" s="123">
         <v>1</v>
       </c>
-      <c r="Q5" s="124"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="R5" s="124"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="31">
         <v>1</v>
       </c>
@@ -5117,24 +5161,27 @@
       <c r="H6" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="39" t="s">
+      <c r="I6" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="52"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="54"/>
-      <c r="N6" s="123">
+      <c r="J6" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="181"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="54"/>
+      <c r="O6" s="123">
         <v>3</v>
       </c>
-      <c r="O6" s="124" t="s">
+      <c r="P6" s="124" t="s">
         <v>182</v>
       </c>
-      <c r="P6" s="123">
+      <c r="Q6" s="123">
         <v>1</v>
       </c>
-      <c r="Q6" s="124"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="R6" s="124"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="33">
         <v>2</v>
       </c>
@@ -5144,22 +5191,23 @@
       <c r="F7" s="42"/>
       <c r="G7" s="49"/>
       <c r="H7" s="42"/>
-      <c r="I7" s="146"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="43"/>
-      <c r="N7" s="123">
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="43"/>
+      <c r="O7" s="123">
         <v>4</v>
       </c>
-      <c r="O7" s="124" t="s">
+      <c r="P7" s="124" t="s">
         <v>183</v>
       </c>
-      <c r="P7" s="123">
+      <c r="Q7" s="123">
         <v>1</v>
       </c>
-      <c r="Q7" s="124"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="R7" s="124"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="33">
         <v>3</v>
       </c>
@@ -5169,22 +5217,23 @@
       <c r="F8" s="42"/>
       <c r="G8" s="49"/>
       <c r="H8" s="42"/>
-      <c r="I8" s="146"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="43"/>
-      <c r="N8" s="96">
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="43"/>
+      <c r="O8" s="96">
         <v>5</v>
       </c>
-      <c r="O8" s="62" t="s">
+      <c r="P8" s="62" t="s">
         <v>184</v>
       </c>
-      <c r="P8" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="62"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q8" s="96">
+        <v>0</v>
+      </c>
+      <c r="R8" s="62"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="33">
         <v>4</v>
       </c>
@@ -5194,22 +5243,23 @@
       <c r="F9" s="42"/>
       <c r="G9" s="49"/>
       <c r="H9" s="42"/>
-      <c r="I9" s="146"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="43"/>
-      <c r="N9" s="123">
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="43"/>
+      <c r="O9" s="123">
         <v>6</v>
       </c>
-      <c r="O9" s="124" t="s">
+      <c r="P9" s="124" t="s">
         <v>185</v>
       </c>
-      <c r="P9" s="123">
+      <c r="Q9" s="123">
         <v>1</v>
       </c>
-      <c r="Q9" s="124"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="R9" s="124"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="33">
         <v>5</v>
       </c>
@@ -5219,22 +5269,23 @@
       <c r="F10" s="42"/>
       <c r="G10" s="49"/>
       <c r="H10" s="42"/>
-      <c r="I10" s="146"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="43"/>
-      <c r="N10" s="123">
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="43"/>
+      <c r="O10" s="123">
         <v>7</v>
       </c>
-      <c r="O10" s="124" t="s">
+      <c r="P10" s="124" t="s">
         <v>186</v>
       </c>
-      <c r="P10" s="123">
+      <c r="Q10" s="123">
         <v>1</v>
       </c>
-      <c r="Q10" s="124"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="R10" s="124"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="33">
         <v>6</v>
       </c>
@@ -5244,26 +5295,27 @@
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
       <c r="H11" s="42"/>
-      <c r="I11" s="146"/>
-      <c r="J11" s="149"/>
-      <c r="K11" s="132"/>
-      <c r="L11" s="134"/>
-      <c r="N11" s="123">
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="131"/>
+      <c r="L11" s="132"/>
+      <c r="M11" s="134"/>
+      <c r="O11" s="123">
         <v>8</v>
       </c>
-      <c r="O11" s="124" t="s">
+      <c r="P11" s="124" t="s">
         <v>187</v>
       </c>
-      <c r="P11" s="123">
+      <c r="Q11" s="123">
         <v>1</v>
       </c>
-      <c r="Q11" s="124"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="167" t="s">
+      <c r="R11" s="124"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="164" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="155"/>
+      <c r="C12" s="152"/>
       <c r="D12" s="62" t="s">
         <v>197</v>
       </c>
@@ -5279,24 +5331,27 @@
       <c r="H12" s="62" t="s">
         <v>215</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="62" t="s">
         <v>217</v>
       </c>
-      <c r="J12" s="139"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="140"/>
-      <c r="N12" s="96">
+      <c r="J12" s="62" t="s">
+        <v>217</v>
+      </c>
+      <c r="K12" s="127"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="140"/>
+      <c r="O12" s="96">
         <v>9</v>
       </c>
-      <c r="O12" s="62" t="s">
+      <c r="P12" s="62" t="s">
         <v>188</v>
       </c>
-      <c r="P12" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="62"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q12" s="96">
+        <v>0</v>
+      </c>
+      <c r="R12" s="62"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="139"/>
       <c r="C13" s="62"/>
       <c r="D13" s="62"/>
@@ -5304,24 +5359,27 @@
       <c r="F13" s="62"/>
       <c r="G13" s="62"/>
       <c r="H13" s="62"/>
-      <c r="I13" s="34" t="s">
+      <c r="I13" s="62" t="s">
         <v>218</v>
       </c>
-      <c r="J13" s="139"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="34"/>
-      <c r="N13" s="96">
+      <c r="J13" s="62" t="s">
+        <v>222</v>
+      </c>
+      <c r="K13" s="127"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="34"/>
+      <c r="O13" s="96">
         <v>10</v>
       </c>
-      <c r="O13" s="62" t="s">
+      <c r="P13" s="62" t="s">
         <v>189</v>
       </c>
-      <c r="P13" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="62"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q13" s="96">
+        <v>0</v>
+      </c>
+      <c r="R13" s="62"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="139"/>
       <c r="C14" s="62"/>
       <c r="D14" s="62"/>
@@ -5329,22 +5387,25 @@
       <c r="F14" s="62"/>
       <c r="G14" s="62"/>
       <c r="H14" s="62"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="139"/>
-      <c r="K14" s="62"/>
-      <c r="L14" s="34"/>
-      <c r="N14" s="96">
+      <c r="I14" s="177"/>
+      <c r="J14" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="K14" s="139"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="34"/>
+      <c r="O14" s="96">
         <v>11</v>
       </c>
-      <c r="O14" s="62" t="s">
+      <c r="P14" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="P14" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="62"/>
-    </row>
-    <row r="15" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q14" s="96">
+        <v>0</v>
+      </c>
+      <c r="R14" s="62"/>
+    </row>
+    <row r="15" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="141"/>
       <c r="C15" s="142"/>
       <c r="D15" s="142"/>
@@ -5352,113 +5413,114 @@
       <c r="F15" s="142"/>
       <c r="G15" s="142"/>
       <c r="H15" s="142"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="141"/>
-      <c r="K15" s="142"/>
-      <c r="L15" s="36"/>
-      <c r="N15" s="96">
+      <c r="I15" s="178"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="141"/>
+      <c r="L15" s="142"/>
+      <c r="M15" s="36"/>
+      <c r="O15" s="96">
         <v>12</v>
       </c>
-      <c r="O15" s="62" t="s">
+      <c r="P15" s="62" t="s">
         <v>191</v>
       </c>
-      <c r="P15" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="62"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="N16" s="96">
+      <c r="Q15" s="96">
+        <v>0</v>
+      </c>
+      <c r="R15" s="62"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O16" s="96">
         <v>13</v>
       </c>
-      <c r="O16" s="62" t="s">
+      <c r="P16" s="62" t="s">
         <v>190</v>
       </c>
-      <c r="P16" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="62"/>
-    </row>
-    <row r="17" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="N17" s="96">
+      <c r="Q16" s="96">
+        <v>0</v>
+      </c>
+      <c r="R16" s="62"/>
+    </row>
+    <row r="17" spans="13:18" x14ac:dyDescent="0.3">
+      <c r="O17" s="96">
         <v>14</v>
       </c>
-      <c r="O17" s="62" t="s">
+      <c r="P17" s="62" t="s">
         <v>192</v>
       </c>
-      <c r="P17" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="62"/>
-    </row>
-    <row r="18" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="N18" s="96">
+      <c r="Q17" s="96">
+        <v>0</v>
+      </c>
+      <c r="R17" s="62"/>
+    </row>
+    <row r="18" spans="13:18" x14ac:dyDescent="0.3">
+      <c r="O18" s="96">
         <v>15</v>
       </c>
-      <c r="O18" s="62" t="s">
+      <c r="P18" s="62" t="s">
         <v>193</v>
       </c>
-      <c r="P18" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="62"/>
-    </row>
-    <row r="19" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="N19" s="123">
+      <c r="Q18" s="96">
+        <v>0</v>
+      </c>
+      <c r="R18" s="62"/>
+    </row>
+    <row r="19" spans="13:18" x14ac:dyDescent="0.3">
+      <c r="O19" s="123">
         <v>16</v>
       </c>
-      <c r="O19" s="124" t="s">
+      <c r="P19" s="124" t="s">
         <v>211</v>
       </c>
-      <c r="P19" s="123">
+      <c r="Q19" s="123">
         <v>1</v>
       </c>
-      <c r="Q19" s="124"/>
-    </row>
-    <row r="21" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="N21" s="96"/>
-      <c r="O21" s="64" t="s">
+      <c r="R19" s="124"/>
+    </row>
+    <row r="21" spans="13:18" x14ac:dyDescent="0.3">
+      <c r="O21" s="96"/>
+      <c r="P21" s="64" t="s">
         <v>161</v>
       </c>
-      <c r="P21" s="125">
-        <f>SUM(P4:P19)</f>
+      <c r="Q21" s="125">
+        <f>SUM(Q4:Q19)</f>
         <v>8</v>
       </c>
-      <c r="Q21" s="62"/>
-    </row>
-    <row r="22" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="N22" s="96"/>
-      <c r="O22" s="64" t="s">
+      <c r="R21" s="62"/>
+    </row>
+    <row r="22" spans="13:18" x14ac:dyDescent="0.3">
+      <c r="O22" s="96"/>
+      <c r="P22" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="P22" s="125">
+      <c r="Q22" s="125">
         <v>16</v>
       </c>
-      <c r="Q22" s="62"/>
-    </row>
-    <row r="23" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="N23" s="96"/>
-      <c r="O23" s="64" t="s">
+      <c r="R22" s="62"/>
+    </row>
+    <row r="23" spans="13:18" x14ac:dyDescent="0.3">
+      <c r="O23" s="96"/>
+      <c r="P23" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="P23" s="125">
-        <f>ROUND((P21/P22)*100,2)</f>
+      <c r="Q23" s="125">
+        <f>ROUND((Q21/Q22)*100,2)</f>
         <v>50</v>
       </c>
-      <c r="Q23" s="62"/>
-    </row>
-    <row r="24" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="L24" t="s">
+      <c r="R23" s="62"/>
+    </row>
+    <row r="24" spans="13:18" x14ac:dyDescent="0.3">
+      <c r="M24" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="K3:M3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B2:I3"/>
+    <mergeCell ref="B2:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5467,10 +5529,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0268C353-496F-4BD6-A7EF-D042619A03C3}">
-  <dimension ref="B1:Q18"/>
+  <dimension ref="B1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5483,61 +5545,64 @@
     <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.109375" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="150" t="s">
+    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="147" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="152"/>
-      <c r="N2" s="98" t="s">
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="149"/>
+      <c r="O2" s="98" t="s">
         <v>145</v>
       </c>
-      <c r="O2" s="97" t="s">
+      <c r="P2" s="97" t="s">
         <v>148</v>
       </c>
-      <c r="P2" s="98" t="s">
+      <c r="Q2" s="98" t="s">
         <v>160</v>
       </c>
-      <c r="Q2" s="97" t="s">
+      <c r="R2" s="97" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="153"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="154"/>
-      <c r="E3" s="154"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="178"/>
+    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
       <c r="J3" s="174"/>
-      <c r="K3" s="175"/>
-      <c r="L3" s="176"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="96"/>
-      <c r="Q3" s="62"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="165" t="s">
+      <c r="K3" s="171"/>
+      <c r="L3" s="172"/>
+      <c r="M3" s="173"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="96"/>
+      <c r="R3" s="62"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="162" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="166" t="s">
+      <c r="C4" s="163" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="128">
@@ -5558,23 +5623,26 @@
       <c r="I4" s="128">
         <v>45279</v>
       </c>
-      <c r="J4" s="143"/>
-      <c r="K4" s="135"/>
-      <c r="L4" s="137"/>
-      <c r="N4" s="123">
+      <c r="J4" s="128">
+        <v>45286</v>
+      </c>
+      <c r="K4" s="143"/>
+      <c r="L4" s="135"/>
+      <c r="M4" s="137"/>
+      <c r="O4" s="123">
         <v>1</v>
       </c>
-      <c r="O4" s="124" t="s">
+      <c r="P4" s="124" t="s">
         <v>172</v>
       </c>
-      <c r="P4" s="123">
+      <c r="Q4" s="123">
         <v>1</v>
       </c>
-      <c r="Q4" s="124"/>
-    </row>
-    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="157"/>
-      <c r="C5" s="159"/>
+      <c r="R4" s="124"/>
+    </row>
+    <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="154"/>
+      <c r="C5" s="156"/>
       <c r="D5" s="61" t="s">
         <v>198</v>
       </c>
@@ -5593,21 +5661,24 @@
       <c r="I5" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="J5" s="144"/>
-      <c r="K5" s="136"/>
-      <c r="L5" s="138"/>
-      <c r="N5" s="123">
+      <c r="J5" s="61" t="s">
+        <v>204</v>
+      </c>
+      <c r="K5" s="144"/>
+      <c r="L5" s="136"/>
+      <c r="M5" s="138"/>
+      <c r="O5" s="123">
         <v>2</v>
       </c>
-      <c r="O5" s="124" t="s">
+      <c r="P5" s="124" t="s">
         <v>173</v>
       </c>
-      <c r="P5" s="123">
+      <c r="Q5" s="123">
         <v>1</v>
       </c>
-      <c r="Q5" s="124"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="R5" s="124"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="31">
         <v>1</v>
       </c>
@@ -5630,21 +5701,24 @@
         <v>47</v>
       </c>
       <c r="I6" s="39"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="43"/>
-      <c r="N6" s="123">
+      <c r="J6" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="41"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="43"/>
+      <c r="O6" s="123">
         <v>3</v>
       </c>
-      <c r="O6" s="124" t="s">
+      <c r="P6" s="124" t="s">
         <v>174</v>
       </c>
-      <c r="P6" s="123">
+      <c r="Q6" s="123">
         <v>1</v>
       </c>
-      <c r="Q6" s="124"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="R6" s="124"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="33">
         <v>2</v>
       </c>
@@ -5655,23 +5729,24 @@
       <c r="G7" s="49"/>
       <c r="H7" s="62"/>
       <c r="I7" s="127"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="43"/>
-      <c r="N7" s="96">
+      <c r="J7" s="127"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="43"/>
+      <c r="O7" s="96">
         <v>4</v>
       </c>
-      <c r="O7" s="62" t="s">
+      <c r="P7" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="P7" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="62" t="s">
+      <c r="Q7" s="96">
+        <v>0</v>
+      </c>
+      <c r="R7" s="62" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="33">
         <v>3</v>
       </c>
@@ -5682,21 +5757,22 @@
       <c r="G8" s="49"/>
       <c r="H8" s="62"/>
       <c r="I8" s="127"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="43"/>
-      <c r="N8" s="123">
+      <c r="J8" s="127"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="43"/>
+      <c r="O8" s="123">
         <v>5</v>
       </c>
-      <c r="O8" s="124" t="s">
+      <c r="P8" s="124" t="s">
         <v>176</v>
       </c>
-      <c r="P8" s="123">
+      <c r="Q8" s="123">
         <v>1</v>
       </c>
-      <c r="Q8" s="124"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="R8" s="124"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="33">
         <v>4</v>
       </c>
@@ -5707,21 +5783,22 @@
       <c r="G9" s="49"/>
       <c r="H9" s="62"/>
       <c r="I9" s="127"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="43"/>
-      <c r="N9" s="96">
+      <c r="J9" s="127"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="43"/>
+      <c r="O9" s="96">
         <v>6</v>
       </c>
-      <c r="O9" s="62" t="s">
+      <c r="P9" s="62" t="s">
         <v>177</v>
       </c>
-      <c r="P9" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="62"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q9" s="96">
+        <v>0</v>
+      </c>
+      <c r="R9" s="62"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="33">
         <v>5</v>
       </c>
@@ -5732,21 +5809,22 @@
       <c r="G10" s="49"/>
       <c r="H10" s="62"/>
       <c r="I10" s="127"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="43"/>
-      <c r="N10" s="96">
+      <c r="J10" s="127"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="43"/>
+      <c r="O10" s="96">
         <v>7</v>
       </c>
-      <c r="O10" s="62" t="s">
+      <c r="P10" s="62" t="s">
         <v>178</v>
       </c>
-      <c r="P10" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="62"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q10" s="96">
+        <v>0</v>
+      </c>
+      <c r="R10" s="62"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="129">
         <v>6</v>
       </c>
@@ -5756,26 +5834,27 @@
       <c r="F11" s="132"/>
       <c r="G11" s="63"/>
       <c r="H11" s="133"/>
-      <c r="I11" s="177"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="43"/>
-      <c r="N11" s="96">
+      <c r="I11" s="146"/>
+      <c r="J11" s="146"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="43"/>
+      <c r="O11" s="96">
         <v>8</v>
       </c>
-      <c r="O11" s="62" t="s">
+      <c r="P11" s="62" t="s">
         <v>179</v>
       </c>
-      <c r="P11" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="62"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="167" t="s">
+      <c r="Q11" s="96">
+        <v>0</v>
+      </c>
+      <c r="R11" s="62"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="164" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="155"/>
+      <c r="C12" s="152"/>
       <c r="D12" s="62" t="s">
         <v>199</v>
       </c>
@@ -5794,21 +5873,24 @@
       <c r="I12" s="127" t="s">
         <v>219</v>
       </c>
-      <c r="J12" s="127"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="140"/>
-      <c r="N12" s="96">
+      <c r="J12" s="127" t="s">
+        <v>199</v>
+      </c>
+      <c r="K12" s="127"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="140"/>
+      <c r="O12" s="96">
         <v>9</v>
       </c>
-      <c r="O12" s="62" t="s">
+      <c r="P12" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="P12" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="62"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q12" s="96">
+        <v>0</v>
+      </c>
+      <c r="R12" s="62"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="139"/>
       <c r="C13" s="62"/>
       <c r="D13" s="62"/>
@@ -5821,21 +5903,24 @@
       <c r="I13" s="127" t="s">
         <v>220</v>
       </c>
-      <c r="J13" s="127"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="34"/>
-      <c r="N13" s="96">
+      <c r="J13" s="127" t="s">
+        <v>224</v>
+      </c>
+      <c r="K13" s="127"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="34"/>
+      <c r="O13" s="96">
         <v>10</v>
       </c>
-      <c r="O13" s="62" t="s">
+      <c r="P13" s="62" t="s">
         <v>195</v>
       </c>
-      <c r="P13" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="62"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q13" s="96">
+        <v>0</v>
+      </c>
+      <c r="R13" s="62"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="139"/>
       <c r="C14" s="62"/>
       <c r="D14" s="62"/>
@@ -5844,21 +5929,24 @@
       <c r="G14" s="62"/>
       <c r="H14" s="62"/>
       <c r="I14" s="127"/>
-      <c r="J14" s="127"/>
-      <c r="K14" s="62"/>
-      <c r="L14" s="34"/>
-      <c r="N14" s="96">
+      <c r="J14" s="127" t="s">
+        <v>225</v>
+      </c>
+      <c r="K14" s="127"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="34"/>
+      <c r="O14" s="96">
         <v>11</v>
       </c>
-      <c r="O14" s="62" t="s">
+      <c r="P14" s="62" t="s">
         <v>196</v>
       </c>
-      <c r="P14" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="62"/>
-    </row>
-    <row r="15" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q14" s="96">
+        <v>0</v>
+      </c>
+      <c r="R14" s="62"/>
+    </row>
+    <row r="15" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="141"/>
       <c r="C15" s="142"/>
       <c r="D15" s="142"/>
@@ -5868,49 +5956,50 @@
       <c r="H15" s="142"/>
       <c r="I15" s="145"/>
       <c r="J15" s="145"/>
-      <c r="K15" s="142"/>
-      <c r="L15" s="36"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="N16" s="96"/>
-      <c r="O16" s="64" t="s">
+      <c r="K15" s="145"/>
+      <c r="L15" s="142"/>
+      <c r="M15" s="36"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O16" s="96"/>
+      <c r="P16" s="64" t="s">
         <v>161</v>
       </c>
-      <c r="P16" s="125">
-        <f>SUM(P4:P14)</f>
+      <c r="Q16" s="125">
+        <f>SUM(Q4:Q14)</f>
         <v>4</v>
       </c>
-      <c r="Q16" s="62"/>
-    </row>
-    <row r="17" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N17" s="96"/>
-      <c r="O17" s="64" t="s">
+      <c r="R16" s="62"/>
+    </row>
+    <row r="17" spans="15:18" x14ac:dyDescent="0.3">
+      <c r="O17" s="96"/>
+      <c r="P17" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="P17" s="125">
-        <f>COUNT(P4:P14)</f>
+      <c r="Q17" s="125">
+        <f>COUNT(Q4:Q14)</f>
         <v>11</v>
       </c>
-      <c r="Q17" s="62"/>
-    </row>
-    <row r="18" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N18" s="96"/>
-      <c r="O18" s="64" t="s">
+      <c r="R17" s="62"/>
+    </row>
+    <row r="18" spans="15:18" x14ac:dyDescent="0.3">
+      <c r="O18" s="96"/>
+      <c r="P18" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="P18" s="125">
-        <f>ROUND((P16/P17)*100,2)</f>
+      <c r="Q18" s="125">
+        <f>ROUND((Q16/Q17)*100,2)</f>
         <v>36.36</v>
       </c>
-      <c r="Q18" s="62"/>
+      <c r="R18" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="K3:M3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B2:I3"/>
+    <mergeCell ref="B2:J3"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>